<commit_message>
JSON and templates updated with functions
</commit_message>
<xml_diff>
--- a/data/final.xlsx
+++ b/data/final.xlsx
@@ -12,8 +12,8 @@
     <sheet name="Subject" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Source" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PredicateObjectMaps" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Functions" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Function_new" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Functions_old" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Functions" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -81,24 +81,15 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">PERSON</t>
-  </si>
-  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/user/data/people.csv</t>
+    <t xml:space="preserve">data/employeds.csv</t>
   </si>
   <si>
     <t xml:space="preserve">format</t>
   </si>
   <si>
-    <t xml:space="preserve">CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/employeds.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">csv</t>
   </si>
   <si>
@@ -222,7 +213,7 @@
     <t xml:space="preserve">grel:valueParameter</t>
   </si>
   <si>
-    <t xml:space="preserve">sport</t>
+    <t xml:space="preserve">{sport}</t>
   </si>
   <si>
     <t xml:space="preserve">grel:p_string_find</t>
@@ -630,7 +621,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="133" zoomScaleNormal="133" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,72 +642,52 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -737,7 +708,7 @@
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B5" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B3" type="list">
       <formula1>"source;format;iterator;table"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -775,22 +746,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>8</v>
@@ -798,13 +769,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -815,13 +786,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -832,13 +803,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -849,7 +820,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -857,10 +828,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
@@ -868,13 +839,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -885,13 +856,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -902,13 +873,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -919,10 +890,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -934,13 +905,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -948,13 +919,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -1003,25 +974,25 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -1037,16 +1008,16 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1082,7 +1053,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,13 +1066,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -1115,13 +1086,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1135,13 +1106,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1155,13 +1126,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1175,13 +1146,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>

</xml_diff>

<commit_message>
stable version without functions
</commit_message>
<xml_diff>
--- a/data/final.xlsx
+++ b/data/final.xlsx
@@ -5,15 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Subject" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Source" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="PredicateObjectMaps" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Functions_old" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Functions" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Functions" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -175,33 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">FunctionID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Param5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sql:upper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grel:valueParameter {sport}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grel:p_string_find “ “</t>
   </si>
   <si>
     <t xml:space="preserve">fno:executes</t>
@@ -958,98 +930,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.97"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -1089,10 +969,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -1109,10 +989,10 @@
         <v>43</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1129,10 +1009,10 @@
         <v>43</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1149,10 +1029,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>

</xml_diff>

<commit_message>
improvement in datatype recognition, imgs deleted
</commit_message>
<xml_diff>
--- a/data/final.xlsx
+++ b/data/final.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -131,7 +131,10 @@
     <t xml:space="preserve">schema:description</t>
   </si>
   <si>
-    <t xml:space="preserve">{bio}</t>
+    <t xml:space="preserve">http://ex.com/{bio}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">anyURI</t>
   </si>
   <si>
     <t xml:space="preserve">schema:image</t>
@@ -171,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">{article}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iri </t>
   </si>
   <si>
     <t xml:space="preserve">FunctionID</t>
@@ -702,8 +708,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -781,7 +787,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -792,7 +798,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -800,10 +806,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>10</v>
@@ -814,7 +820,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>31</v>
@@ -828,10 +834,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>31</v>
@@ -845,10 +851,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>31</v>
@@ -862,10 +868,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -876,28 +882,28 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -915,6 +921,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="http://ex.com/{bio}"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -932,7 +941,7 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -946,7 +955,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>23</v>
@@ -966,13 +975,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -986,13 +995,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1006,13 +1015,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
@@ -1026,13 +1035,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>

</xml_diff>